<commit_message>
Added statement for not storing image
</commit_message>
<xml_diff>
--- a/Statlog.xlsx
+++ b/Statlog.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="326">
   <si>
     <t>N</t>
   </si>
@@ -895,6 +895,96 @@
   </si>
   <si>
     <t>ConnTime_end</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>StartUp</t>
+  </si>
+  <si>
+    <t>FindTime</t>
+  </si>
+  <si>
+    <t>ConnTime_start</t>
+  </si>
+  <si>
+    <t>ConnTime_end</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime_start</t>
+  </si>
+  <si>
+    <t>ConnTime_end</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime_start</t>
+  </si>
+  <si>
+    <t>ConnTime_end</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime_start</t>
+  </si>
+  <si>
+    <t>ConnTime_end</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime_start</t>
+  </si>
+  <si>
+    <t>ConnTime_end</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
   </si>
   <si>
     <t>ResetTime</t>
@@ -921,7 +1011,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -936,11 +1026,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -949,6 +1040,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,27 +1061,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>270</v>
+        <v>296</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>271</v>
+        <v>297</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>272</v>
+        <v>298</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>295</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="8">
         <v>44270.473286030094</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>273</v>
+        <v>299</v>
       </c>
       <c r="D2" s="0">
         <v>0</v>
@@ -999,11 +1091,11 @@
       <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="8">
         <v>44270.473286035733</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>274</v>
+        <v>300</v>
       </c>
       <c r="D3" s="0">
         <v>2.2255124999999998</v>
@@ -1013,11 +1105,11 @@
       <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="8">
         <v>44270.473311967595</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>275</v>
+        <v>301</v>
       </c>
       <c r="D4" s="0">
         <v>0</v>
@@ -1027,11 +1119,11 @@
       <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="8">
         <v>44270.473311980459</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>276</v>
+        <v>302</v>
       </c>
       <c r="D5" s="0">
         <v>11.9358883</v>
@@ -1041,11 +1133,11 @@
       <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="8">
         <v>44270.47363057582</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>277</v>
+        <v>303</v>
       </c>
       <c r="D6" s="0">
         <v>3.0162491999999999</v>
@@ -1055,11 +1147,11 @@
       <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="8">
         <v>44270.473665615209</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>278</v>
+        <v>304</v>
       </c>
       <c r="D7" s="0">
         <v>0.72484579999999998</v>
@@ -1069,11 +1161,11 @@
       <c r="A8" s="0">
         <v>7</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="8">
         <v>44270.473674618057</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="D8" s="0">
         <v>0</v>
@@ -1083,11 +1175,11 @@
       <c r="A9" s="0">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="8">
         <v>44270.473674667999</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="D9" s="0">
         <v>12.230684699999999</v>
@@ -1097,11 +1189,11 @@
       <c r="A10" s="0">
         <v>9</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="8">
         <v>44270.473674740497</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
       <c r="D10" s="0">
         <v>17.245420800000002</v>
@@ -1111,11 +1203,11 @@
       <c r="A11" s="0">
         <v>10</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="8">
         <v>44270.473941477234</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>282</v>
+        <v>308</v>
       </c>
       <c r="D11" s="0">
         <v>2.0333668999999999</v>
@@ -1125,11 +1217,11 @@
       <c r="A12" s="0">
         <v>11</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="8">
         <v>44270.473965018333</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>283</v>
+        <v>309</v>
       </c>
       <c r="D12" s="0">
         <v>0.68741600000000003</v>
@@ -1139,11 +1231,11 @@
       <c r="A13" s="0">
         <v>12</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="8">
         <v>44270.473973518521</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>284</v>
+        <v>310</v>
       </c>
       <c r="D13" s="0">
         <v>0</v>
@@ -1153,11 +1245,11 @@
       <c r="A14" s="0">
         <v>13</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="8">
         <v>44270.473973477114</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>285</v>
+        <v>311</v>
       </c>
       <c r="D14" s="0">
         <v>11.727576900000001</v>
@@ -1167,11 +1259,11 @@
       <c r="A15" s="0">
         <v>14</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="8">
         <v>44270.473973601744</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="D15" s="0">
         <v>16.742809000000001</v>
@@ -1181,11 +1273,11 @@
       <c r="A16" s="0">
         <v>15</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="8">
         <v>44270.475010891205</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>287</v>
+        <v>313</v>
       </c>
       <c r="D16" s="0">
         <v>0</v>
@@ -1195,11 +1287,11 @@
       <c r="A17" s="0">
         <v>16</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="8">
         <v>44270.475010928196</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>288</v>
+        <v>314</v>
       </c>
       <c r="D17" s="0">
         <v>12.201803399999999</v>
@@ -1209,11 +1301,11 @@
       <c r="A18" s="0">
         <v>17</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="8">
         <v>44270.475010977207</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>289</v>
+        <v>315</v>
       </c>
       <c r="D18" s="0">
         <v>17.2145692</v>
@@ -1223,11 +1315,11 @@
       <c r="A19" s="0">
         <v>18</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="8">
         <v>44270.475904818974</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>290</v>
+        <v>316</v>
       </c>
       <c r="D19" s="0">
         <v>1.9696408000000001</v>
@@ -1237,11 +1329,11 @@
       <c r="A20" s="0">
         <v>19</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="8">
         <v>44270.475927755702</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c r="D20" s="0">
         <v>0.58890690000000001</v>
@@ -1251,11 +1343,11 @@
       <c r="A21" s="0">
         <v>20</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="8">
         <v>44270.47593497685</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>292</v>
+        <v>318</v>
       </c>
       <c r="D21" s="0">
         <v>0</v>
@@ -1265,11 +1357,11 @@
       <c r="A22" s="0">
         <v>21</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="8">
         <v>44270.475935043316</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>293</v>
+        <v>319</v>
       </c>
       <c r="D22" s="0">
         <v>11.561257899999999</v>
@@ -1279,11 +1371,11 @@
       <c r="A23" s="0">
         <v>22</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="8">
         <v>44270.475935068665</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>294</v>
+        <v>320</v>
       </c>
       <c r="D23" s="0">
         <v>16.575067600000001</v>
@@ -1293,56 +1385,56 @@
       <c r="A24" s="0">
         <v>23</v>
       </c>
-      <c r="B24" s="6">
-        <v>44270.462141026364</v>
+      <c r="B24" s="8">
+        <v>44270.476821837336</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>244</v>
+        <v>321</v>
       </c>
       <c r="D24" s="0">
-        <v>17.097322200000001</v>
+        <v>2.0442542000000001</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
         <v>24</v>
       </c>
-      <c r="B25" s="6">
-        <v>44270.46372809507</v>
+      <c r="B25" s="8">
+        <v>44270.476845528465</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>245</v>
+        <v>322</v>
       </c>
       <c r="D25" s="0">
-        <v>3.1225855999999999</v>
+        <v>0.63934100000000005</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
         <v>25</v>
       </c>
-      <c r="B26" s="6">
-        <v>44270.463764268672</v>
+      <c r="B26" s="8">
+        <v>44270.47685413561</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>246</v>
+        <v>323</v>
       </c>
       <c r="D26" s="0">
-        <v>0.69818630000000004</v>
+        <v>11.1906836</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
         <v>26</v>
       </c>
-      <c r="B27" s="6">
-        <v>44270.463773587966</v>
+      <c r="B27" s="8">
+        <v>44270.476854131281</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>247</v>
+        <v>324</v>
       </c>
       <c r="D27" s="0">
-        <v>0</v>
+        <v>16.2050576</v>
       </c>
     </row>
     <row r="28">

</xml_diff>

<commit_message>
Some changes to camera obj
</commit_message>
<xml_diff>
--- a/Statlog.xlsx
+++ b/Statlog.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7083" uniqueCount="7083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7817" uniqueCount="7817">
   <si>
     <t>N</t>
   </si>
@@ -21253,6 +21253,2208 @@
   </si>
   <si>
     <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>StartUp</t>
+  </si>
+  <si>
+    <t>FindTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>StartUp</t>
+  </si>
+  <si>
+    <t>FindTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>StartUp</t>
+  </si>
+  <si>
+    <t>FindTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>StartUp</t>
+  </si>
+  <si>
+    <t>FindTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>StartUp</t>
+  </si>
+  <si>
+    <t>FindTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>StartUp</t>
+  </si>
+  <si>
+    <t>FindTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>StartUp</t>
+  </si>
+  <si>
+    <t>FindTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>StartUp</t>
+  </si>
+  <si>
+    <t>FindTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>StartUp</t>
+  </si>
+  <si>
+    <t>FindTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTime</t>
+  </si>
+  <si>
+    <t>StoreTime</t>
+  </si>
+  <si>
+    <t>ResetTime</t>
+  </si>
+  <si>
+    <t>ConnTime</t>
+  </si>
+  <si>
+    <t>ShootTimeError</t>
   </si>
   <si>
     <t>ResetTime</t>
@@ -21282,7 +23484,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="104">
+  <borders count="113">
     <border>
       <left/>
       <right/>
@@ -21393,11 +23595,20 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -21502,6 +23713,15 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="101" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="102" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="103" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="104" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="105" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="106" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="109" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="110" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="111" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="112" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -21522,27 +23742,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>7021</v>
+        <v>7721</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7022</v>
+        <v>7722</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>7023</v>
+        <v>7723</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>7082</v>
+        <v>7816</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" s="103">
+      <c r="B2" s="112">
         <v>44270.598012557872</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7024</v>
+        <v>7724</v>
       </c>
       <c r="D2" s="0">
         <v>0</v>
@@ -21552,11 +23772,11 @@
       <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" s="103">
+      <c r="B3" s="112">
         <v>44270.598013792587</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>7025</v>
+        <v>7725</v>
       </c>
       <c r="D3" s="0">
         <v>2.2833203000000002</v>
@@ -21566,11 +23786,11 @@
       <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" s="103">
+      <c r="B4" s="112">
         <v>44270.598041311554</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>7026</v>
+        <v>7726</v>
       </c>
       <c r="D4" s="0">
         <v>12.622681699999999</v>
@@ -21580,11 +23800,11 @@
       <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" s="103">
+      <c r="B5" s="112">
         <v>44270.598220118954</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>7027</v>
+        <v>7727</v>
       </c>
       <c r="D5" s="0">
         <v>1.5947221</v>
@@ -21594,11 +23814,11 @@
       <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" s="103">
+      <c r="B6" s="112">
         <v>44270.598239335341</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>7028</v>
+        <v>7728</v>
       </c>
       <c r="D6" s="0">
         <v>15.918427100000001</v>
@@ -21608,11 +23828,11 @@
       <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" s="103">
+      <c r="B7" s="112">
         <v>44270.598426511628</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>7029</v>
+        <v>7729</v>
       </c>
       <c r="D7" s="0">
         <v>11.974395700000001</v>
@@ -21622,11 +23842,11 @@
       <c r="A8" s="0">
         <v>7</v>
       </c>
-      <c r="B8" s="103">
+      <c r="B8" s="112">
         <v>44270.598426670891</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>7030</v>
+        <v>7730</v>
       </c>
       <c r="D8" s="0">
         <v>12.0166346</v>
@@ -21636,11 +23856,11 @@
       <c r="A9" s="0">
         <v>8</v>
       </c>
-      <c r="B9" s="103">
+      <c r="B9" s="112">
         <v>44270.599990417839</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>7031</v>
+        <v>7731</v>
       </c>
       <c r="D9" s="0">
         <v>4.1278988999999999</v>
@@ -21650,11 +23870,11 @@
       <c r="A10" s="0">
         <v>9</v>
       </c>
-      <c r="B10" s="103">
+      <c r="B10" s="112">
         <v>44270.600039904639</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>7032</v>
+        <v>7732</v>
       </c>
       <c r="D10" s="0">
         <v>16.5762392</v>
@@ -21664,11 +23884,11 @@
       <c r="A11" s="0">
         <v>10</v>
       </c>
-      <c r="B11" s="103">
+      <c r="B11" s="112">
         <v>44270.600235152851</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>7033</v>
+        <v>7733</v>
       </c>
       <c r="D11" s="0">
         <v>12.4127937</v>
@@ -21678,11 +23898,11 @@
       <c r="A12" s="0">
         <v>11</v>
       </c>
-      <c r="B12" s="103">
+      <c r="B12" s="112">
         <v>44270.600235117134</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>7034</v>
+        <v>7734</v>
       </c>
       <c r="D12" s="0">
         <v>12.4158802</v>
@@ -21692,11 +23912,11 @@
       <c r="A13" s="0">
         <v>12</v>
       </c>
-      <c r="B13" s="103">
+      <c r="B13" s="112">
         <v>44270.601379094784</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>7035</v>
+        <v>7735</v>
       </c>
       <c r="D13" s="0">
         <v>1.5332110999999999</v>
@@ -21706,11 +23926,11 @@
       <c r="A14" s="0">
         <v>13</v>
       </c>
-      <c r="B14" s="103">
+      <c r="B14" s="112">
         <v>44270.601396873528</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>7036</v>
+        <v>7736</v>
       </c>
       <c r="D14" s="0">
         <v>15.416126999999999</v>
@@ -21720,11 +23940,11 @@
       <c r="A15" s="0">
         <v>14</v>
       </c>
-      <c r="B15" s="103">
+      <c r="B15" s="112">
         <v>44270.601577218687</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>7037</v>
+        <v>7737</v>
       </c>
       <c r="D15" s="0">
         <v>12.180305799999999</v>
@@ -21734,11 +23954,11 @@
       <c r="A16" s="0">
         <v>15</v>
       </c>
-      <c r="B16" s="103">
+      <c r="B16" s="112">
         <v>44270.601577212867</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>7038</v>
+        <v>7738</v>
       </c>
       <c r="D16" s="0">
         <v>12.182808700000001</v>
@@ -21748,11 +23968,11 @@
       <c r="A17" s="0">
         <v>16</v>
       </c>
-      <c r="B17" s="103">
+      <c r="B17" s="112">
         <v>44270.602767907512</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>7039</v>
+        <v>7739</v>
       </c>
       <c r="D17" s="0">
         <v>1.5777908</v>
@@ -21762,11 +23982,11 @@
       <c r="A18" s="0">
         <v>17</v>
       </c>
-      <c r="B18" s="103">
+      <c r="B18" s="112">
         <v>44270.602786314899</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>7040</v>
+        <v>7740</v>
       </c>
       <c r="D18" s="0">
         <v>14.749392800000001</v>
@@ -21776,11 +23996,11 @@
       <c r="A19" s="0">
         <v>18</v>
       </c>
-      <c r="B19" s="103">
+      <c r="B19" s="112">
         <v>44270.603023036078</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>7041</v>
+        <v>7741</v>
       </c>
       <c r="D19" s="0">
         <v>12.341683</v>
@@ -21790,11 +24010,11 @@
       <c r="A20" s="0">
         <v>19</v>
       </c>
-      <c r="B20" s="103">
+      <c r="B20" s="112">
         <v>44270.603023030875</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>7042</v>
+        <v>7742</v>
       </c>
       <c r="D20" s="0">
         <v>12.3451323</v>
@@ -21804,11 +24024,11 @@
       <c r="A21" s="0">
         <v>20</v>
       </c>
-      <c r="B21" s="103">
+      <c r="B21" s="112">
         <v>44270.604156648275</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>7043</v>
+        <v>7743</v>
       </c>
       <c r="D21" s="0">
         <v>1.5725891999999999</v>
@@ -21818,11 +24038,11 @@
       <c r="A22" s="0">
         <v>21</v>
       </c>
-      <c r="B22" s="103">
+      <c r="B22" s="112">
         <v>44270.604174910724</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>7044</v>
+        <v>7744</v>
       </c>
       <c r="D22" s="0">
         <v>14.992713500000001</v>
@@ -21832,11 +24052,11 @@
       <c r="A23" s="0">
         <v>22</v>
       </c>
-      <c r="B23" s="103">
+      <c r="B23" s="112">
         <v>44270.60435257067</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>7045</v>
+        <v>7745</v>
       </c>
       <c r="D23" s="0">
         <v>12.335894100000001</v>
@@ -21846,11 +24066,11 @@
       <c r="A24" s="0">
         <v>23</v>
       </c>
-      <c r="B24" s="103">
+      <c r="B24" s="112">
         <v>44270.604352507056</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>7046</v>
+        <v>7746</v>
       </c>
       <c r="D24" s="0">
         <v>12.3413907</v>
@@ -21860,11 +24080,11 @@
       <c r="A25" s="0">
         <v>24</v>
       </c>
-      <c r="B25" s="103">
+      <c r="B25" s="112">
         <v>44270.605545549144</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>7047</v>
+        <v>7747</v>
       </c>
       <c r="D25" s="0">
         <v>10.4715536</v>
@@ -21874,11 +24094,11 @@
       <c r="A26" s="0">
         <v>25</v>
       </c>
-      <c r="B26" s="103">
+      <c r="B26" s="112">
         <v>44270.605666902375</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>7048</v>
+        <v>7748</v>
       </c>
       <c r="D26" s="0">
         <v>10.592635100000001</v>
@@ -21888,11 +24108,11 @@
       <c r="A27" s="0">
         <v>26</v>
       </c>
-      <c r="B27" s="103">
+      <c r="B27" s="112">
         <v>44270.605667044532</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>7049</v>
+        <v>7749</v>
       </c>
       <c r="D27" s="0">
         <v>10.595352800000001</v>
@@ -21902,11 +24122,11 @@
       <c r="A28" s="0">
         <v>27</v>
       </c>
-      <c r="B28" s="103">
+      <c r="B28" s="112">
         <v>44270.60693442246</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>7050</v>
+        <v>7750</v>
       </c>
       <c r="D28" s="0">
         <v>9.9418994999999999</v>
@@ -21916,11 +24136,11 @@
       <c r="A29" s="0">
         <v>28</v>
       </c>
-      <c r="B29" s="103">
+      <c r="B29" s="112">
         <v>44270.607049490682</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>7051</v>
+        <v>7751</v>
       </c>
       <c r="D29" s="0">
         <v>22.567004600000001</v>
@@ -21930,11 +24150,11 @@
       <c r="A30" s="0">
         <v>29</v>
       </c>
-      <c r="B30" s="103">
+      <c r="B30" s="112">
         <v>44270.607311414198</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>7052</v>
+        <v>7752</v>
       </c>
       <c r="D30" s="0">
         <v>11.994813000000001</v>
@@ -21944,11 +24164,11 @@
       <c r="A31" s="0">
         <v>30</v>
       </c>
-      <c r="B31" s="103">
+      <c r="B31" s="112">
         <v>44270.607311419742</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>7053</v>
+        <v>7753</v>
       </c>
       <c r="D31" s="0">
         <v>11.9993338</v>
@@ -21958,11 +24178,11 @@
       <c r="A32" s="0">
         <v>31</v>
       </c>
-      <c r="B32" s="103">
+      <c r="B32" s="112">
         <v>44270.608323330307</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>7054</v>
+        <v>7754</v>
       </c>
       <c r="D32" s="0">
         <v>1.5222614999999999</v>
@@ -21972,11 +24192,11 @@
       <c r="A33" s="0">
         <v>32</v>
       </c>
-      <c r="B33" s="103">
+      <c r="B33" s="112">
         <v>44270.608340944993</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>7055</v>
+        <v>7755</v>
       </c>
       <c r="D33" s="0">
         <v>14.4463528</v>
@@ -21986,11 +24206,11 @@
       <c r="A34" s="0">
         <v>33</v>
       </c>
-      <c r="B34" s="103">
+      <c r="B34" s="112">
         <v>44270.608511936996</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>7056</v>
+        <v>7756</v>
       </c>
       <c r="D34" s="0">
         <v>12.0696437</v>
@@ -22000,11 +24220,11 @@
       <c r="A35" s="0">
         <v>34</v>
       </c>
-      <c r="B35" s="103">
+      <c r="B35" s="112">
         <v>44270.608511938364</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>7057</v>
+        <v>7757</v>
       </c>
       <c r="D35" s="0">
         <v>12.073525099999999</v>
@@ -22014,11 +24234,11 @@
       <c r="A36" s="0">
         <v>35</v>
       </c>
-      <c r="B36" s="103">
+      <c r="B36" s="112">
         <v>44270.609712149599</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>7058</v>
+        <v>7758</v>
       </c>
       <c r="D36" s="0">
         <v>3.1322747</v>
@@ -22028,11 +24248,11 @@
       <c r="A37" s="0">
         <v>36</v>
       </c>
-      <c r="B37" s="103">
+      <c r="B37" s="112">
         <v>44270.609748577372</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>7059</v>
+        <v>7759</v>
       </c>
       <c r="D37" s="0">
         <v>15.7509151</v>
@@ -22042,11 +24262,11 @@
       <c r="A38" s="0">
         <v>37</v>
       </c>
-      <c r="B38" s="103">
+      <c r="B38" s="112">
         <v>44270.609930939536</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>7060</v>
+        <v>7760</v>
       </c>
       <c r="D38" s="0">
         <v>0.060824099999999999</v>
@@ -22056,11 +24276,11 @@
       <c r="A39" s="0">
         <v>38</v>
       </c>
-      <c r="B39" s="103">
+      <c r="B39" s="112">
         <v>44270.609931562431</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>7061</v>
+        <v>7761</v>
       </c>
       <c r="D39" s="0">
         <v>12.212006000000001</v>
@@ -22070,11 +24290,11 @@
       <c r="A40" s="0">
         <v>39</v>
       </c>
-      <c r="B40" s="103">
+      <c r="B40" s="112">
         <v>44270.611101105729</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>7062</v>
+        <v>7762</v>
       </c>
       <c r="D40" s="0">
         <v>1.5294645</v>
@@ -22084,11 +24304,11 @@
       <c r="A41" s="0">
         <v>40</v>
       </c>
-      <c r="B41" s="103">
+      <c r="B41" s="112">
         <v>44270.61111887946</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>7063</v>
+        <v>7763</v>
       </c>
       <c r="D41" s="0">
         <v>14.264814100000001</v>
@@ -22098,11 +24318,11 @@
       <c r="A42" s="0">
         <v>41</v>
       </c>
-      <c r="B42" s="103">
+      <c r="B42" s="112">
         <v>44270.61128404487</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>7064</v>
+        <v>7764</v>
       </c>
       <c r="D42" s="0">
         <v>0.075523199999999999</v>
@@ -22112,11 +24332,11 @@
       <c r="A43" s="0">
         <v>42</v>
       </c>
-      <c r="B43" s="103">
+      <c r="B43" s="112">
         <v>44270.611284821854</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>7065</v>
+        <v>7765</v>
       </c>
       <c r="D43" s="0">
         <v>12.2353919</v>
@@ -22126,11 +24346,11 @@
       <c r="A44" s="0">
         <v>43</v>
       </c>
-      <c r="B44" s="103">
+      <c r="B44" s="112">
         <v>44270.612490003725</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>7066</v>
+        <v>7766</v>
       </c>
       <c r="D44" s="0">
         <v>1.5016783</v>
@@ -22140,11 +24360,11 @@
       <c r="A45" s="0">
         <v>44</v>
       </c>
-      <c r="B45" s="103">
+      <c r="B45" s="112">
         <v>44270.612507275298</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>7067</v>
+        <v>7767</v>
       </c>
       <c r="D45" s="0">
         <v>13.5914138</v>
@@ -22154,11 +24374,11 @@
       <c r="A46" s="0">
         <v>45</v>
       </c>
-      <c r="B46" s="103">
+      <c r="B46" s="112">
         <v>44270.612664737964</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>7068</v>
+        <v>7768</v>
       </c>
       <c r="D46" s="0">
         <v>0.11364</v>
@@ -22168,11 +24388,11 @@
       <c r="A47" s="0">
         <v>46</v>
       </c>
-      <c r="B47" s="103">
+      <c r="B47" s="112">
         <v>44270.612666150242</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>7069</v>
+        <v>7769</v>
       </c>
       <c r="D47" s="0">
         <v>11.8106189</v>
@@ -22182,11 +24402,11 @@
       <c r="A48" s="0">
         <v>47</v>
       </c>
-      <c r="B48" s="103">
+      <c r="B48" s="112">
         <v>44270.613878814831</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>7070</v>
+        <v>7770</v>
       </c>
       <c r="D48" s="0">
         <v>1.5153984</v>
@@ -22196,11 +24416,11 @@
       <c r="A49" s="0">
         <v>48</v>
       </c>
-      <c r="B49" s="103">
+      <c r="B49" s="112">
         <v>44270.613896404771</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>7071</v>
+        <v>7771</v>
       </c>
       <c r="D49" s="0">
         <v>15.9146278</v>
@@ -22210,11 +24430,11 @@
       <c r="A50" s="0">
         <v>49</v>
       </c>
-      <c r="B50" s="103">
+      <c r="B50" s="112">
         <v>44270.614080664411</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>7072</v>
+        <v>7772</v>
       </c>
       <c r="D50" s="0">
         <v>0.075594499999999995</v>
@@ -22224,11 +24444,11 @@
       <c r="A51" s="0">
         <v>50</v>
       </c>
-      <c r="B51" s="103">
+      <c r="B51" s="112">
         <v>44270.614081573214</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>7073</v>
+        <v>7773</v>
       </c>
       <c r="D51" s="0">
         <v>12.080074400000001</v>
@@ -22238,11 +24458,11 @@
       <c r="A52" s="0">
         <v>51</v>
       </c>
-      <c r="B52" s="103">
+      <c r="B52" s="112">
         <v>44270.615267735644</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>7074</v>
+        <v>7774</v>
       </c>
       <c r="D52" s="0">
         <v>1.5826408000000001</v>
@@ -22252,11 +24472,11 @@
       <c r="A53" s="0">
         <v>52</v>
       </c>
-      <c r="B53" s="103">
+      <c r="B53" s="112">
         <v>44270.615286116845</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>7075</v>
+        <v>7775</v>
       </c>
       <c r="D53" s="0">
         <v>18.8595048</v>
@@ -22266,11 +24486,11 @@
       <c r="A54" s="0">
         <v>53</v>
       </c>
-      <c r="B54" s="103">
+      <c r="B54" s="112">
         <v>44270.615504464033</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>7076</v>
+        <v>7776</v>
       </c>
       <c r="D54" s="0">
         <v>0.27130739999999998</v>
@@ -22280,11 +24500,11 @@
       <c r="A55" s="0">
         <v>54</v>
       </c>
-      <c r="B55" s="103">
+      <c r="B55" s="112">
         <v>44270.615507508439</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>7077</v>
+        <v>7777</v>
       </c>
       <c r="D55" s="0">
         <v>11.779271100000001</v>
@@ -22294,11 +24514,11 @@
       <c r="A56" s="0">
         <v>55</v>
       </c>
-      <c r="B56" s="103">
+      <c r="B56" s="112">
         <v>44270.616656611608</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>7078</v>
+        <v>7778</v>
       </c>
       <c r="D56" s="0">
         <v>5.699757</v>
@@ -22308,11 +24528,11 @@
       <c r="A57" s="0">
         <v>56</v>
       </c>
-      <c r="B57" s="103">
+      <c r="B57" s="112">
         <v>44270.616722557257</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>7079</v>
+        <v>7779</v>
       </c>
       <c r="D57" s="0">
         <v>15.4590532</v>
@@ -22322,11 +24542,11 @@
       <c r="A58" s="0">
         <v>57</v>
       </c>
-      <c r="B58" s="103">
+      <c r="B58" s="112">
         <v>44270.616930349504</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>7080</v>
+        <v>7780</v>
       </c>
       <c r="D58" s="0">
         <v>0.094802600000000001</v>
@@ -22336,11 +24556,11 @@
       <c r="A59" s="0">
         <v>58</v>
       </c>
-      <c r="B59" s="103">
+      <c r="B59" s="112">
         <v>44270.616931548822</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>7081</v>
+        <v>7781</v>
       </c>
       <c r="D59" s="0">
         <v>12.4761819</v>
@@ -22350,476 +24570,476 @@
       <c r="A60" s="0">
         <v>59</v>
       </c>
-      <c r="B60" s="65">
-        <v>44270.535177778307</v>
+      <c r="B60" s="112">
+        <v>44270.618045479772</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>5671</v>
+        <v>7782</v>
       </c>
       <c r="D60" s="0">
-        <v>6.8759543000000001</v>
+        <v>9.7475474999999996</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0">
         <v>60</v>
       </c>
-      <c r="B61" s="65">
-        <v>44270.535257362819</v>
+      <c r="B61" s="112">
+        <v>44270.618158346049</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>5672</v>
+        <v>7783</v>
       </c>
       <c r="D61" s="0">
-        <v>20.137852500000001</v>
+        <v>18.4709015</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0">
         <v>61</v>
       </c>
-      <c r="B62" s="65">
-        <v>44270.535493199939</v>
+      <c r="B62" s="112">
+        <v>44270.618372230754</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>5673</v>
+        <v>7784</v>
       </c>
       <c r="D62" s="0">
-        <v>11.727525200000001</v>
+        <v>0.2062629</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0">
         <v>62</v>
       </c>
-      <c r="B63" s="65">
-        <v>44270.535493342046</v>
+      <c r="B63" s="112">
+        <v>44270.618374500627</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>5674</v>
+        <v>7785</v>
       </c>
       <c r="D63" s="0">
-        <v>16.742247200000001</v>
+        <v>12.238146</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0">
         <v>63</v>
       </c>
-      <c r="B64" s="65">
-        <v>44270.536382019556</v>
+      <c r="B64" s="112">
+        <v>44270.61943446668</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>5675</v>
+        <v>7786</v>
       </c>
       <c r="D64" s="0">
-        <v>1.6055102999999999</v>
+        <v>1.5670789000000001</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0">
         <v>64</v>
       </c>
-      <c r="B65" s="65">
-        <v>44270.53640060898</v>
+      <c r="B65" s="112">
+        <v>44270.619452643819</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>5676</v>
+        <v>7787</v>
       </c>
       <c r="D65" s="0">
-        <v>15.8903839</v>
+        <v>14.5465745</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0">
         <v>65</v>
       </c>
-      <c r="B66" s="65">
-        <v>44270.536589102368</v>
+      <c r="B66" s="112">
+        <v>44270.619621079553</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>5677</v>
+        <v>7788</v>
       </c>
       <c r="D66" s="0">
-        <v>11.4515557</v>
+        <v>0.26372620000000002</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0">
         <v>66</v>
       </c>
-      <c r="B67" s="65">
-        <v>44270.536589108764</v>
+      <c r="B67" s="112">
+        <v>44270.61962407206</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>5678</v>
+        <v>7789</v>
       </c>
       <c r="D67" s="0">
-        <v>16.464002799999999</v>
+        <v>12.3051735</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0">
         <v>67</v>
       </c>
-      <c r="B68" s="65">
-        <v>44270.537474388846</v>
+      <c r="B68" s="112">
+        <v>44270.620823193123</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>5679</v>
+        <v>7790</v>
       </c>
       <c r="D68" s="0">
-        <v>10.460803500000001</v>
+        <v>2.6051142999999999</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0">
         <v>68</v>
       </c>
-      <c r="B69" s="65">
-        <v>44270.537595787071</v>
+      <c r="B69" s="112">
+        <v>44270.62085340386</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>5680</v>
+        <v>7791</v>
       </c>
       <c r="D69" s="0">
-        <v>12.062996800000001</v>
+        <v>16.756906499999999</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0">
         <v>69</v>
       </c>
-      <c r="B70" s="65">
-        <v>44270.537595817717</v>
+      <c r="B70" s="112">
+        <v>44270.621047427201</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>5681</v>
+        <v>7792</v>
       </c>
       <c r="D70" s="0">
-        <v>17.075349200000002</v>
+        <v>0.1202898</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0">
         <v>70</v>
       </c>
-      <c r="B71" s="65">
-        <v>44270.538488014528</v>
+      <c r="B71" s="112">
+        <v>44270.621048963949</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>5682</v>
+        <v>7793</v>
       </c>
       <c r="D71" s="0">
-        <v>1.5985448</v>
+        <v>11.254514500000001</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0">
         <v>71</v>
       </c>
-      <c r="B72" s="65">
-        <v>44270.538506688768</v>
+      <c r="B72" s="112">
+        <v>44270.622212032344</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>5683</v>
+        <v>7794</v>
       </c>
       <c r="D72" s="0">
-        <v>14.4070903</v>
+        <v>2.2324058</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0">
         <v>72</v>
       </c>
-      <c r="B73" s="65">
-        <v>44270.538682790393</v>
+      <c r="B73" s="112">
+        <v>44270.622238030417</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>5684</v>
+        <v>7795</v>
       </c>
       <c r="D73" s="0">
-        <v>11.846910400000001</v>
+        <v>15.451172</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0">
         <v>73</v>
       </c>
-      <c r="B74" s="65">
-        <v>44270.538682941078</v>
+      <c r="B74" s="112">
+        <v>44270.622416932194</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>5685</v>
+        <v>7796</v>
       </c>
       <c r="D74" s="0">
-        <v>16.858891199999999</v>
+        <v>0.19205839999999999</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0">
         <v>74</v>
       </c>
-      <c r="B75" s="65">
-        <v>44270.539572660964</v>
+      <c r="B75" s="112">
+        <v>44270.622419200678</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>5686</v>
+        <v>7797</v>
       </c>
       <c r="D75" s="0">
-        <v>10.307093099999999</v>
+        <v>12.1070612</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0">
         <v>75</v>
       </c>
-      <c r="B76" s="65">
-        <v>44270.539692269725</v>
+      <c r="B76" s="112">
+        <v>44270.623600879473</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>5687</v>
+        <v>7798</v>
       </c>
       <c r="D76" s="0">
-        <v>11.9138956</v>
+        <v>2.0850140000000001</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0">
         <v>76</v>
       </c>
-      <c r="B77" s="65">
-        <v>44270.539692334794</v>
+      <c r="B77" s="112">
+        <v>44270.623625206536</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>5688</v>
+        <v>7799</v>
       </c>
       <c r="D77" s="0">
-        <v>16.924274</v>
+        <v>13.910155100000001</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0">
         <v>77</v>
       </c>
-      <c r="B78" s="49">
-        <v>44270.490270099137</v>
+      <c r="B78" s="112">
+        <v>44270.623786275202</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>4683</v>
+        <v>7800</v>
       </c>
       <c r="D78" s="0">
-        <v>1.3004344999999999</v>
+        <v>0.52682200000000001</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0">
         <v>78</v>
       </c>
-      <c r="B79" s="49">
-        <v>44270.49028606958</v>
+      <c r="B79" s="112">
+        <v>44270.623792276056</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>4684</v>
+        <v>7801</v>
       </c>
       <c r="D79" s="0">
-        <v>11.907588499999999</v>
+        <v>11.3633487</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0">
         <v>79</v>
       </c>
-      <c r="B80" s="49">
-        <v>44270.490286168453</v>
+      <c r="B80" s="112">
+        <v>44270.624989934593</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>4685</v>
+        <v>7802</v>
       </c>
       <c r="D80" s="0">
-        <v>16.9190456</v>
+        <v>2.5296509999999999</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0">
         <v>80</v>
       </c>
-      <c r="B81" s="49">
-        <v>44270.491176738069</v>
+      <c r="B81" s="112">
+        <v>44270.625019363324</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>4686</v>
+        <v>7803</v>
       </c>
       <c r="D81" s="0">
-        <v>2.0348307999999999</v>
+        <v>15.4120089</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0">
         <v>81</v>
       </c>
-      <c r="B82" s="49">
-        <v>44270.491200206539</v>
+      <c r="B82" s="112">
+        <v>44270.625197831825</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>4687</v>
+        <v>7804</v>
       </c>
       <c r="D82" s="0">
-        <v>0.67215469999999999</v>
+        <v>0.1363299</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0">
         <v>82</v>
       </c>
-      <c r="B83" s="49">
-        <v>44270.491208581458</v>
+      <c r="B83" s="112">
+        <v>44270.625199472284</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>4688</v>
+        <v>7805</v>
       </c>
       <c r="D83" s="0">
-        <v>12.107562</v>
+        <v>11.547594699999999</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0">
         <v>83</v>
       </c>
-      <c r="B84" s="49">
-        <v>44270.491208748674</v>
+      <c r="B84" s="112">
+        <v>44270.626378796173</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>4689</v>
+        <v>7806</v>
       </c>
       <c r="D84" s="0">
-        <v>17.119114700000001</v>
+        <v>0.029010399999999999</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0">
         <v>84</v>
       </c>
-      <c r="B85" s="49">
-        <v>44270.492101779833</v>
+      <c r="B85" s="112">
+        <v>44270.626379189038</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>4690</v>
+        <v>7807</v>
       </c>
       <c r="D85" s="0">
-        <v>10.275222899999999</v>
+        <v>0.0150671</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0">
         <v>85</v>
       </c>
-      <c r="B86" s="49">
-        <v>44270.49222090104</v>
+      <c r="B86" s="112">
+        <v>44270.626379383873</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>4691</v>
+        <v>7808</v>
       </c>
       <c r="D86" s="0">
-        <v>11.700150499999999</v>
+        <v>11.1412335</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0">
         <v>86</v>
       </c>
-      <c r="B87" s="49">
-        <v>44270.49222100366</v>
+      <c r="B87" s="112">
+        <v>44270.6277677244</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>4692</v>
+        <v>7809</v>
       </c>
       <c r="D87" s="0">
-        <v>16.712283599999999</v>
+        <v>1.5976117000000001</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0">
         <v>87</v>
       </c>
-      <c r="B88" s="49">
-        <v>44270.493109235707</v>
+      <c r="B88" s="112">
+        <v>44270.627786268989</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>4693</v>
+        <v>7810</v>
       </c>
       <c r="D88" s="0">
-        <v>3.0230350000000001</v>
+        <v>16.275359600000002</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0">
         <v>88</v>
       </c>
-      <c r="B89" s="49">
-        <v>44270.493144333799</v>
+      <c r="B89" s="112">
+        <v>44270.627974702147</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>4694</v>
+        <v>7811</v>
       </c>
       <c r="D89" s="0">
-        <v>0.69855979999999995</v>
+        <v>0.091734300000000005</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0">
         <v>89</v>
       </c>
-      <c r="B90" s="49">
-        <v>44270.493153208372</v>
+      <c r="B90" s="112">
+        <v>44270.627975816664</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>4695</v>
+        <v>7812</v>
       </c>
       <c r="D90" s="0">
-        <v>12.2877969</v>
+        <v>11.282440100000001</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0">
         <v>90</v>
       </c>
-      <c r="B91" s="49">
-        <v>44270.493153280913</v>
+      <c r="B91" s="112">
+        <v>44270.629156587864</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>4696</v>
+        <v>7813</v>
       </c>
       <c r="D91" s="0">
-        <v>17.302528800000001</v>
+        <v>10.357808800000001</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0">
         <v>91</v>
       </c>
-      <c r="B92" s="49">
-        <v>44270.494048364984</v>
+      <c r="B92" s="112">
+        <v>44270.629276460801</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>4697</v>
+        <v>7814</v>
       </c>
       <c r="D92" s="0">
-        <v>1.9682656999999999</v>
+        <v>0.015786499999999998</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0">
         <v>92</v>
       </c>
-      <c r="B93" s="49">
-        <v>44270.494071132322</v>
+      <c r="B93" s="112">
+        <v>44270.629276689331</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>4698</v>
+        <v>7815</v>
       </c>
       <c r="D93" s="0">
-        <v>0.63216749999999999</v>
+        <v>11.3650419</v>
       </c>
     </row>
     <row r="94">

</xml_diff>